<commit_message>
Ajustes gerais e ícones
</commit_message>
<xml_diff>
--- a/Tabela_Icone.xlsx
+++ b/Tabela_Icone.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24703"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24709"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2DECCAF3-B4C8-4FF6-B3B0-DC4A8FFD9B8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{97576E9B-60C9-43E4-92DC-AEB758B5BC9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="109">
   <si>
     <t>Função</t>
   </si>
@@ -50,7 +50,10 @@
     <t>Padrão</t>
   </si>
   <si>
-    <t>fal fa-ad</t>
+    <t>fal fa-font-case, fal fa-id-card-alt, fal fa-id-badge</t>
+  </si>
+  <si>
+    <t>fal fa-audio-description</t>
   </si>
   <si>
     <t>Usuário</t>
@@ -177,6 +180,42 @@
   </si>
   <si>
     <t>fal fa-user-graduate</t>
+  </si>
+  <si>
+    <t>Type (gateway)</t>
+  </si>
+  <si>
+    <t>fal fa-torii-gate</t>
+  </si>
+  <si>
+    <t>gateway_sip_user</t>
+  </si>
+  <si>
+    <t>fal fa-user-md-chat</t>
+  </si>
+  <si>
+    <t>gateway_ext</t>
+  </si>
+  <si>
+    <t>fal fa-apple-crate</t>
+  </si>
+  <si>
+    <t>gateway_domain</t>
+  </si>
+  <si>
+    <t>fal fa-landmark</t>
+  </si>
+  <si>
+    <t>IP</t>
+  </si>
+  <si>
+    <t>fal fa-ellipsis-h-alt</t>
+  </si>
+  <si>
+    <t>Importar arquivo</t>
+  </si>
+  <si>
+    <t>fal fa-file-upload</t>
   </si>
   <si>
     <t>Ramal</t>
@@ -783,53 +822,6 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>295275</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagem 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E1099BD-732D-4ECC-B137-25EA6C32C787}"/>
-            </a:ext>
-            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{F3E8B1DE-4914-4439-9240-8303D11C846E}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="4714875" y="200025"/>
-          <a:ext cx="342900" cy="285750"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
       <xdr:colOff>200025</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
@@ -857,7 +849,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -904,7 +896,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -951,7 +943,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -998,7 +990,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1019,13 +1011,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>781050</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>409575</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1045,7 +1037,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1066,13 +1058,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>628650</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>27</xdr:row>
       <xdr:rowOff>361950</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1092,7 +1084,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1113,13 +1105,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>742950</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>352425</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1139,7 +1131,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1160,13 +1152,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>400050</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1186,7 +1178,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1207,13 +1199,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>742950</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>361950</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1233,7 +1225,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1254,13 +1246,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>457200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1280,7 +1272,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1301,13 +1293,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>762000</xdr:colOff>
-      <xdr:row>30</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>304800</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1327,7 +1319,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1348,13 +1340,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>704850</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>295275</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1374,7 +1366,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1395,13 +1387,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>32</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>266700</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1421,7 +1413,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1442,13 +1434,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>39</xdr:row>
       <xdr:rowOff>381000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1468,7 +1460,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1489,13 +1481,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>504825</xdr:colOff>
-      <xdr:row>34</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>276225</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1515,7 +1507,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1562,7 +1554,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1609,7 +1601,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1656,7 +1648,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1703,7 +1695,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1750,7 +1742,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1797,7 +1789,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1844,7 +1836,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1891,7 +1883,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1938,7 +1930,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -1959,13 +1951,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>57150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>26</xdr:row>
       <xdr:rowOff>447675</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1985,7 +1977,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId26"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2006,13 +1998,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>438150</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2032,7 +2024,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2053,13 +2045,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>104775</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>381000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2079,7 +2071,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId28"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2126,7 +2118,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId24"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2173,7 +2165,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2194,13 +2186,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>26</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>457200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2220,7 +2212,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId30"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2267,7 +2259,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2314,7 +2306,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId33"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId32"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2361,7 +2353,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId34"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId33"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2408,7 +2400,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId35"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId34"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2429,229 +2421,652 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>457200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="69" name="Imagem 68">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59E100E4-1A57-475A-90DC-27BA22790AAD}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{40442FF2-D6A4-4DFE-BD1C-E8AB8923F878}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId35"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11496675" y="9353550"/>
+          <a:ext cx="390525" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>409575</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="70" name="Imagem 69">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C4F8BDF6-310B-4AC5-AE76-6F55E3BBD04F}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{59E100E4-1A57-475A-90DC-27BA22790AAD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId36"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11458575" y="9877425"/>
+          <a:ext cx="390525" cy="314325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>438150</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="71" name="Imagem 70">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A3E5B52-0541-4CFA-8AF3-52F32E00A93F}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{C4F8BDF6-310B-4AC5-AE76-6F55E3BBD04F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId37"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11496675" y="10353675"/>
+          <a:ext cx="371475" cy="371475"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>438150</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="72" name="Imagem 46">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6745551-49A0-4CEE-973F-7E2EC207A19D}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{4A3E5B52-0541-4CFA-8AF3-52F32E00A93F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId22"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5791200" y="6324600"/>
+          <a:ext cx="419100" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>371475</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Imagem 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2680FF82-B648-47FB-AFE0-EB003FD0AD89}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{D6745551-49A0-4CEE-973F-7E2EC207A19D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId38"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6238875" y="9410700"/>
+          <a:ext cx="333375" cy="295275"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>361950</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Imagem 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DEEF9D10-5BBD-42B8-97FD-8FD2ABFC551F}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{2680FF82-B648-47FB-AFE0-EB003FD0AD89}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId39"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6772275" y="304800"/>
+          <a:ext cx="295275" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>657225</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>314325</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Imagem 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEABD0D4-461F-4EF1-BEC4-523E5B66654D}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{DEEF9D10-5BBD-42B8-97FD-8FD2ABFC551F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId40"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7096125" y="314325"/>
+          <a:ext cx="285750" cy="247650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>704850</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1057275</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>438150</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Imagem 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{958004EE-D504-4A4C-9768-206ACFA87E98}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{AEABD0D4-461F-4EF1-BEC4-523E5B66654D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId41"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7429500" y="266700"/>
+          <a:ext cx="352425" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>438150</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Imagem 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E821AE03-7EDE-46D0-97FC-8D122E0D8DF0}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{958004EE-D504-4A4C-9768-206ACFA87E98}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId42"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8829675" y="9372600"/>
+          <a:ext cx="285750" cy="400050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>714375</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>438150</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Imagem 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E4AEE97-4C0C-41C4-8712-2E17107B5892}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{E821AE03-7EDE-46D0-97FC-8D122E0D8DF0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId43"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8877300" y="9372600"/>
+          <a:ext cx="381000" cy="400050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>752475</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>419100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Imagem 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87005F7B-FCB8-45DD-A833-7EDAC889520B}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{1E4AEE97-4C0C-41C4-8712-2E17107B5892}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId44"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8867775" y="10439400"/>
+          <a:ext cx="428625" cy="323850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>657225</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>409575</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Imagem 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FF0DB69D-E7DC-43D3-A0B8-036296B98254}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{87005F7B-FCB8-45DD-A833-7EDAC889520B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId45"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8867775" y="9867900"/>
+          <a:ext cx="333375" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>771525</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>476250</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Imagem 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08494FD6-77B0-4096-99BC-6E16EA8E81B1}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{FF0DB69D-E7DC-43D3-A0B8-036296B98254}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId46"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8829675" y="9858375"/>
+          <a:ext cx="485775" cy="457200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
       <xdr:row>20</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>457200</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="69" name="Imagem 68">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59E100E4-1A57-475A-90DC-27BA22790AAD}"/>
-            </a:ext>
-            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{40442FF2-D6A4-4DFE-BD1C-E8AB8923F878}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId36"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11496675" y="9353550"/>
-          <a:ext cx="390525" cy="381000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>514350</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>409575</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="70" name="Imagem 69">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C4F8BDF6-310B-4AC5-AE76-6F55E3BBD04F}"/>
-            </a:ext>
-            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{59E100E4-1A57-475A-90DC-27BA22790AAD}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId37"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11458575" y="9877425"/>
-          <a:ext cx="390525" cy="314325"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>438150</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="71" name="Imagem 70">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A3E5B52-0541-4CFA-8AF3-52F32E00A93F}"/>
-            </a:ext>
-            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{C4F8BDF6-310B-4AC5-AE76-6F55E3BBD04F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId38"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="11496675" y="10353675"/>
-          <a:ext cx="371475" cy="371475"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>438150</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="72" name="Imagem 46">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6745551-49A0-4CEE-973F-7E2EC207A19D}"/>
-            </a:ext>
-            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{4A3E5B52-0541-4CFA-8AF3-52F32E00A93F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="5791200" y="6324600"/>
-          <a:ext cx="419100" cy="419100"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>666750</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>371475</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Imagem 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2680FF82-B648-47FB-AFE0-EB003FD0AD89}"/>
-            </a:ext>
-            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{D6745551-49A0-4CEE-973F-7E2EC207A19D}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId39"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="6238875" y="9410700"/>
-          <a:ext cx="333375" cy="295275"/>
+      <xdr:rowOff>428625</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Imagem 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1029F023-A1A7-4546-BA2A-7536ABF78E38}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{08494FD6-77B0-4096-99BC-6E16EA8E81B1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId47"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8848725" y="9915525"/>
+          <a:ext cx="419100" cy="352425"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3139,8 +3554,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{18CD4719-C934-4F77-B68A-69EC9F18F93C}" name="Tabela2" displayName="Tabela2" ref="A1:E36" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A1:E36" xr:uid="{18CD4719-C934-4F77-B68A-69EC9F18F93C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{18CD4719-C934-4F77-B68A-69EC9F18F93C}" name="Tabela2" displayName="Tabela2" ref="A1:E42" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:E42" xr:uid="{18CD4719-C934-4F77-B68A-69EC9F18F93C}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{AB7B4547-9008-478E-8B1B-566C4A9E50A0}" name="Função"/>
     <tableColumn id="2" xr3:uid="{BB6739B7-E7BA-46AF-BF21-12047FD5C362}" name="Tipo" dataDxfId="3"/>
@@ -3449,17 +3864,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M36"/>
+  <dimension ref="A1:M42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.28515625" bestFit="1" customWidth="1"/>
@@ -3492,174 +3907,176 @@
       <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="4"/>
+      <c r="C2" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="D2" s="6" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E2" s="4"/>
     </row>
     <row r="3" spans="1:13" ht="39.75" customHeight="1">
       <c r="A3" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E3" s="4"/>
     </row>
     <row r="4" spans="1:13" ht="39.75" customHeight="1">
       <c r="A4" s="4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E4" s="4"/>
     </row>
     <row r="5" spans="1:13" ht="39.75" customHeight="1">
       <c r="A5" s="4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E5" s="4"/>
     </row>
     <row r="6" spans="1:13" ht="39.75" customHeight="1">
       <c r="A6" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E6" s="4"/>
     </row>
     <row r="7" spans="1:13" ht="39.75" customHeight="1">
       <c r="A7" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E7" s="4"/>
     </row>
     <row r="8" spans="1:13" ht="39.75" customHeight="1">
       <c r="A8" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="6" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E8" s="4"/>
     </row>
     <row r="9" spans="1:13" ht="39.75" customHeight="1">
       <c r="A9" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="6" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E9" s="4"/>
     </row>
     <row r="10" spans="1:13" ht="39.75" customHeight="1">
       <c r="A10" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E10" s="4"/>
     </row>
     <row r="11" spans="1:13" ht="39.75" customHeight="1">
       <c r="A11" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="6" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E11" s="4"/>
     </row>
     <row r="12" spans="1:13" ht="39.75" customHeight="1">
       <c r="A12" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="6" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E12" s="4"/>
     </row>
     <row r="13" spans="1:13" ht="39.75" customHeight="1">
       <c r="A13" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="6" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E13" s="4"/>
     </row>
     <row r="14" spans="1:13" ht="39.75" customHeight="1">
       <c r="A14" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="6" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E14" s="4"/>
     </row>
     <row r="15" spans="1:13" ht="39.75" customHeight="1">
       <c r="A15" s="7" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="8"/>
@@ -3682,111 +4099,111 @@
     </row>
     <row r="16" spans="1:13" ht="39.75" customHeight="1">
       <c r="A16" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="6" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="E16" s="4"/>
       <c r="I16" s="15" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J16" s="15" t="s">
         <v>6</v>
       </c>
       <c r="K16" s="15"/>
       <c r="L16" s="17" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="M16" s="15"/>
     </row>
     <row r="17" spans="1:13" ht="39.75" customHeight="1">
       <c r="A17" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E17" s="4"/>
       <c r="I17" s="15" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="J17" s="15" t="s">
         <v>6</v>
       </c>
       <c r="K17" s="15"/>
       <c r="L17" s="17" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="M17" s="15"/>
     </row>
     <row r="18" spans="1:13" ht="39.75" customHeight="1">
       <c r="A18" s="4" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E18" s="4"/>
       <c r="I18" s="18" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="J18" s="18" t="s">
         <v>6</v>
       </c>
       <c r="K18" s="18"/>
       <c r="L18" s="18" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M18" s="18"/>
     </row>
     <row r="19" spans="1:13" ht="39.75" customHeight="1">
       <c r="A19" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D19" s="6"/>
       <c r="E19" s="4"/>
       <c r="I19" s="15" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J19" s="18" t="s">
         <v>6</v>
       </c>
       <c r="K19" s="15"/>
       <c r="L19" s="15" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="M19" s="15"/>
     </row>
     <row r="20" spans="1:13" ht="39.75" customHeight="1">
       <c r="A20" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="10"/>
-      <c r="D20" s="6" t="s">
-        <v>51</v>
-      </c>
+      <c r="C20" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D20" s="6"/>
       <c r="E20" s="4"/>
       <c r="I20" s="15"/>
       <c r="J20" s="18"/>
@@ -3796,141 +4213,159 @@
     </row>
     <row r="21" spans="1:13" ht="39.75" customHeight="1">
       <c r="A21" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="4" t="s">
-        <v>53</v>
+      <c r="C21" s="10" t="s">
+        <v>54</v>
       </c>
       <c r="D21" s="6"/>
       <c r="E21" s="4"/>
-      <c r="I21" s="15" t="s">
-        <v>54</v>
-      </c>
-      <c r="J21" s="18" t="s">
-        <v>6</v>
-      </c>
+      <c r="I21" s="15"/>
+      <c r="J21" s="18"/>
       <c r="K21" s="15"/>
-      <c r="L21" s="15" t="s">
-        <v>55</v>
-      </c>
+      <c r="L21" s="15"/>
       <c r="M21" s="15"/>
     </row>
     <row r="22" spans="1:13" ht="39.75" customHeight="1">
       <c r="A22" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C22" s="10" t="s">
         <v>56</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>57</v>
       </c>
       <c r="D22" s="6"/>
       <c r="E22" s="4"/>
-      <c r="I22" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="J22" s="18" t="s">
-        <v>6</v>
-      </c>
+      <c r="I22" s="15"/>
+      <c r="J22" s="18"/>
       <c r="K22" s="15"/>
-      <c r="L22" s="15" t="s">
-        <v>59</v>
-      </c>
+      <c r="L22" s="15"/>
       <c r="M22" s="15"/>
     </row>
     <row r="23" spans="1:13" ht="39.75" customHeight="1">
       <c r="A23" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="4" t="s">
-        <v>61</v>
+      <c r="C23" s="10" t="s">
+        <v>58</v>
       </c>
       <c r="D23" s="6"/>
       <c r="E23" s="4"/>
-      <c r="I23" s="19" t="s">
-        <v>6</v>
-      </c>
-      <c r="J23" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="K23" s="20"/>
-      <c r="L23" s="15" t="s">
-        <v>62</v>
-      </c>
+      <c r="I23" s="15"/>
+      <c r="J23" s="18"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="15"/>
       <c r="M23" s="15"/>
     </row>
     <row r="24" spans="1:13" ht="39.75" customHeight="1">
       <c r="A24" s="4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>64</v>
+      <c r="C24" s="10" t="s">
+        <v>60</v>
       </c>
       <c r="D24" s="6"/>
       <c r="E24" s="4"/>
-      <c r="H24" s="1"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="15"/>
+      <c r="L24" s="15"/>
+      <c r="M24" s="15"/>
     </row>
     <row r="25" spans="1:13" ht="39.75" customHeight="1">
       <c r="A25" s="4" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C25" s="4" t="s">
-        <v>66</v>
+      <c r="C25" s="10" t="s">
+        <v>62</v>
       </c>
       <c r="D25" s="6"/>
       <c r="E25" s="4"/>
+      <c r="I25" s="15"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="15"/>
+      <c r="L25" s="15"/>
+      <c r="M25" s="15"/>
     </row>
     <row r="26" spans="1:13" ht="39.75" customHeight="1">
       <c r="A26" s="4" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C26" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D26" s="6"/>
+      <c r="C26" s="10"/>
+      <c r="D26" s="6" t="s">
+        <v>64</v>
+      </c>
       <c r="E26" s="4"/>
+      <c r="I26" s="15"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="15"/>
+      <c r="L26" s="15"/>
+      <c r="M26" s="15"/>
     </row>
     <row r="27" spans="1:13" ht="39.75" customHeight="1">
       <c r="A27" s="4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="6" t="s">
-        <v>70</v>
-      </c>
+      <c r="C27" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D27" s="6"/>
       <c r="E27" s="4"/>
+      <c r="I27" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="J27" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="K27" s="15"/>
+      <c r="L27" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="M27" s="15"/>
     </row>
     <row r="28" spans="1:13" ht="39.75" customHeight="1">
       <c r="A28" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C28" s="5" t="s">
-        <v>72</v>
+      <c r="C28" s="4" t="s">
+        <v>70</v>
       </c>
       <c r="D28" s="6"/>
       <c r="E28" s="4"/>
+      <c r="I28" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="J28" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="K28" s="15"/>
+      <c r="L28" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="M28" s="15"/>
     </row>
     <row r="29" spans="1:13" ht="39.75" customHeight="1">
       <c r="A29" s="4" t="s">
@@ -3944,97 +4379,187 @@
       </c>
       <c r="D29" s="6"/>
       <c r="E29" s="4"/>
+      <c r="I29" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="J29" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="K29" s="20"/>
+      <c r="L29" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="M29" s="15"/>
     </row>
     <row r="30" spans="1:13" ht="39.75" customHeight="1">
       <c r="A30" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C30" s="5" t="s">
-        <v>76</v>
+      <c r="C30" s="4" t="s">
+        <v>77</v>
       </c>
       <c r="D30" s="6"/>
       <c r="E30" s="4"/>
+      <c r="H30" s="1"/>
     </row>
     <row r="31" spans="1:13" ht="39.75" customHeight="1">
       <c r="A31" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D31" s="6"/>
       <c r="E31" s="4"/>
     </row>
     <row r="32" spans="1:13" ht="39.75" customHeight="1">
-      <c r="A32" s="9" t="s">
-        <v>79</v>
+      <c r="A32" s="4" t="s">
+        <v>80</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>9</v>
+        <v>81</v>
       </c>
       <c r="D32" s="6"/>
       <c r="E32" s="4"/>
     </row>
     <row r="33" spans="1:5" ht="39.75" customHeight="1">
-      <c r="A33" s="11" t="s">
-        <v>80</v>
+      <c r="A33" s="4" t="s">
+        <v>82</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C33" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="D33" s="6"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="6" t="s">
+        <v>83</v>
+      </c>
       <c r="E33" s="4"/>
     </row>
     <row r="34" spans="1:5" ht="39.75" customHeight="1">
-      <c r="A34" s="12" t="s">
-        <v>82</v>
+      <c r="A34" s="4" t="s">
+        <v>84</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C34" s="14" t="s">
-        <v>83</v>
+      <c r="C34" s="5" t="s">
+        <v>85</v>
       </c>
       <c r="D34" s="6"/>
       <c r="E34" s="4"/>
     </row>
     <row r="35" spans="1:5" ht="39.75" customHeight="1">
-      <c r="A35" s="36" t="s">
-        <v>84</v>
+      <c r="A35" s="4" t="s">
+        <v>86</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>6</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D35" s="6"/>
       <c r="E35" s="4"/>
     </row>
-    <row r="36" spans="1:5" ht="38.25" customHeight="1">
-      <c r="A36" s="13" t="s">
-        <v>30</v>
+    <row r="36" spans="1:5" ht="39.75" customHeight="1">
+      <c r="A36" s="4" t="s">
+        <v>88</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C36" s="4"/>
-      <c r="D36" s="6" t="s">
+      <c r="C36" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D36" s="6"/>
+      <c r="E36" s="4"/>
+    </row>
+    <row r="37" spans="1:5" ht="39.75" customHeight="1">
+      <c r="A37" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="D37" s="6"/>
+      <c r="E37" s="4"/>
+    </row>
+    <row r="38" spans="1:5" ht="39.75" customHeight="1">
+      <c r="A38" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D38" s="6"/>
+      <c r="E38" s="4"/>
+    </row>
+    <row r="39" spans="1:5" ht="39.75" customHeight="1">
+      <c r="A39" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D39" s="6"/>
+      <c r="E39" s="4"/>
+    </row>
+    <row r="40" spans="1:5" ht="39.75" customHeight="1">
+      <c r="A40" s="12" t="s">
+        <v>95</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="D40" s="6"/>
+      <c r="E40" s="4"/>
+    </row>
+    <row r="41" spans="1:5" ht="39.75" customHeight="1">
+      <c r="A41" s="36" t="s">
+        <v>97</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D41" s="6"/>
+      <c r="E41" s="4"/>
+    </row>
+    <row r="42" spans="1:5" ht="38.25" customHeight="1">
+      <c r="A42" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="E36" s="4"/>
+      <c r="B42" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C42" s="4"/>
+      <c r="D42" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E42" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -4087,7 +4612,7 @@
       </c>
       <c r="C2" s="27"/>
       <c r="D2" s="32" t="s">
-        <v>86</v>
+        <v>99</v>
       </c>
       <c r="E2" s="28"/>
     </row>
@@ -4098,7 +4623,7 @@
       </c>
       <c r="C3" s="30"/>
       <c r="D3" s="33" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="E3" s="31"/>
     </row>
@@ -4109,7 +4634,7 @@
       </c>
       <c r="C4" s="27"/>
       <c r="D4" s="32" t="s">
-        <v>88</v>
+        <v>101</v>
       </c>
       <c r="E4" s="28"/>
     </row>
@@ -4120,7 +4645,7 @@
       </c>
       <c r="C5" s="30"/>
       <c r="D5" s="33" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="E5" s="31"/>
     </row>
@@ -4131,7 +4656,7 @@
       </c>
       <c r="C6" s="27"/>
       <c r="D6" s="32" t="s">
-        <v>90</v>
+        <v>103</v>
       </c>
       <c r="E6" s="28"/>
     </row>
@@ -4142,7 +4667,7 @@
       </c>
       <c r="C7" s="30"/>
       <c r="D7" s="33" t="s">
-        <v>91</v>
+        <v>104</v>
       </c>
       <c r="E7" s="31"/>
     </row>
@@ -4153,7 +4678,7 @@
       </c>
       <c r="C8" s="27"/>
       <c r="D8" s="32" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="E8" s="28"/>
     </row>
@@ -4164,7 +4689,7 @@
       </c>
       <c r="C9" s="30"/>
       <c r="D9" s="33" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="E9" s="31"/>
     </row>
@@ -4175,7 +4700,7 @@
       </c>
       <c r="C10" s="27"/>
       <c r="D10" s="32" t="s">
-        <v>94</v>
+        <v>107</v>
       </c>
       <c r="E10" s="28"/>
     </row>
@@ -4186,7 +4711,7 @@
       </c>
       <c r="C11" s="34"/>
       <c r="D11" s="34" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="E11" s="3"/>
     </row>

</xml_diff>